<commit_message>
added build_building_table.py, turning index_base into index.html
</commit_message>
<xml_diff>
--- a/Civ7Data.xlsx
+++ b/Civ7Data.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\git\Civ7CheatSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409A4C7E-32BC-470B-9539-7976E84431C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66960519-AB27-46D8-8B19-484E3B2B7DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="12200" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>Building</t>
   </si>
@@ -33,16 +44,124 @@
     <t>Age</t>
   </si>
   <si>
-    <t>production cost</t>
-  </si>
-  <si>
-    <t>base income</t>
-  </si>
-  <si>
-    <t>adjacency Bonus</t>
-  </si>
-  <si>
-    <t>Bonus to improvements</t>
+    <t>INN</t>
+  </si>
+  <si>
+    <t>Exploration</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>UNIVERSITY</t>
+  </si>
+  <si>
+    <t>+5 science</t>
+  </si>
+  <si>
+    <t>+1 science to quarters</t>
+  </si>
+  <si>
+    <t>BRICKYARD</t>
+  </si>
+  <si>
+    <t>+1 production</t>
+  </si>
+  <si>
+    <t>+1 production to Clay Pits, Mines, and Quarries</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>ProductionCost</t>
+  </si>
+  <si>
+    <t>AdjacencyBonus</t>
+  </si>
+  <si>
+    <t>BonusTo</t>
+  </si>
+  <si>
+    <t>PruchaseInTowns</t>
+  </si>
+  <si>
+    <t>BaseYield</t>
+  </si>
+  <si>
+    <t>+3 food +2 happiness</t>
+  </si>
+  <si>
+    <t>+1 food for adjacent: coastal terrain, navigable river terrain, wonder</t>
+  </si>
+  <si>
+    <t>+1 science for adjacent: ressource, wonder</t>
+  </si>
+  <si>
+    <t>Ageless</t>
+  </si>
+  <si>
+    <t>GRISTMILL</t>
+  </si>
+  <si>
+    <t>+4 food</t>
+  </si>
+  <si>
+    <t>+1 food to Farms, Pastures, and Plantations</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Must be placed on a river</t>
+  </si>
+  <si>
+    <t>GUILDHALL</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>+2 influence +4 gold</t>
+  </si>
+  <si>
+    <t>+1 gold for adjacent: coastal terrain, navigable river terrain, wonder</t>
+  </si>
+  <si>
+    <t>OBSERVATORY</t>
+  </si>
+  <si>
+    <t>+4 science</t>
+  </si>
+  <si>
+    <t>SAW PIT</t>
+  </si>
+  <si>
+    <t>+1 production to Camps, Woodcutters</t>
+  </si>
+  <si>
+    <t>SAW MILL</t>
+  </si>
+  <si>
+    <t>+3 production</t>
+  </si>
+  <si>
+    <t>SHIPYARD</t>
+  </si>
+  <si>
+    <t>+5 production</t>
+  </si>
+  <si>
+    <t>+1 production for adjacent: ressource, wonder</t>
+  </si>
+  <si>
+    <t>Must be placed on coast adjacent to land</t>
+  </si>
+  <si>
+    <t>+10% production towards Naval Units</t>
   </si>
 </sst>
 </file>
@@ -78,8 +197,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -360,40 +480,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G2"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A11" sqref="A11:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="26.6328125" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" customWidth="1"/>
-    <col min="6" max="6" width="21.1796875" customWidth="1"/>
-    <col min="7" max="7" width="22.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="26.6328125" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="63.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="37.08984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>55</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>175</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>175</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated building table xls with new data
</commit_message>
<xml_diff>
--- a/Civ7Data.xlsx
+++ b/Civ7Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\git\Civ7CheatSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66960519-AB27-46D8-8B19-484E3B2B7DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A241C93D-1646-4B4D-B024-CAEEC28AD939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD31"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added sorting at buidling table import
</commit_message>
<xml_diff>
--- a/Civ7Data.xlsx
+++ b/Civ7Data.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\git\Civ7CheatSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A241C93D-1646-4B4D-B024-CAEEC28AD939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E667AAE-8C31-4A89-A1B3-CA5DBC7F1A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="12200" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>Building</t>
   </si>
@@ -162,6 +165,36 @@
   </si>
   <si>
     <t>+10% production towards Naval Units</t>
+  </si>
+  <si>
+    <t>GRANARY</t>
+  </si>
+  <si>
+    <t>+1 food</t>
+  </si>
+  <si>
+    <t>GARDEN</t>
+  </si>
+  <si>
+    <t>Antiquity</t>
+  </si>
+  <si>
+    <t>+3 food</t>
+  </si>
+  <si>
+    <t>1+ food for adjacent: coastal terrain, navigable river terrain, wonder</t>
+  </si>
+  <si>
+    <t>ALTAR</t>
+  </si>
+  <si>
+    <t>+2 happiness</t>
+  </si>
+  <si>
+    <t>+1 happiness for adjacent: wonder</t>
+  </si>
+  <si>
+    <t>Recieves additional bonuses from Pantheon</t>
   </si>
 </sst>
 </file>
@@ -480,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,53 +559,56 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C2">
-        <v>200</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C3">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -587,7 +623,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -595,7 +631,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -604,13 +640,13 @@
         <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>26</v>
@@ -621,42 +657,43 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <f>55*320/220</f>
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>4</v>
@@ -667,22 +704,26 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C8">
-        <v>55</v>
+        <f>55*360/220</f>
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>34</v>
+        <v>4</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>11</v>
@@ -690,54 +731,128 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
+        <v>200</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more buildings to list
</commit_message>
<xml_diff>
--- a/Civ7Data.xlsx
+++ b/Civ7Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\git\Civ7CheatSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E667AAE-8C31-4A89-A1B3-CA5DBC7F1A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5D66A5-E259-4258-A178-7305660F6858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25710" yWindow="12200" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="77">
   <si>
     <t>Building</t>
   </si>
@@ -128,9 +128,6 @@
     <t>???</t>
   </si>
   <si>
-    <t>+2 influence +4 gold</t>
-  </si>
-  <si>
     <t>+1 gold for adjacent: coastal terrain, navigable river terrain, wonder</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>+1 production to Camps, Woodcutters</t>
   </si>
   <si>
-    <t>SAW MILL</t>
-  </si>
-  <si>
     <t>+3 production</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>Must be placed on coast adjacent to land</t>
   </si>
   <si>
-    <t>+10% production towards Naval Units</t>
-  </si>
-  <si>
     <t>GRANARY</t>
   </si>
   <si>
@@ -195,6 +186,90 @@
   </si>
   <si>
     <t>Recieves additional bonuses from Pantheon</t>
+  </si>
+  <si>
+    <t>MARKET</t>
+  </si>
+  <si>
+    <t>+2 gold</t>
+  </si>
+  <si>
+    <t>BATH</t>
+  </si>
+  <si>
+    <t>MONUMENT</t>
+  </si>
+  <si>
+    <t>+2 culture +1 influence</t>
+  </si>
+  <si>
+    <t>+1 culture for adjacent: mountain, natural wonder, wonder</t>
+  </si>
+  <si>
+    <t>BARRACKS</t>
+  </si>
+  <si>
+    <t>+2 production</t>
+  </si>
+  <si>
+    <t>+10% production towards naval units</t>
+  </si>
+  <si>
+    <t>+10% production towards land units</t>
+  </si>
+  <si>
+    <t>+10% growth rate</t>
+  </si>
+  <si>
+    <t>VILLA</t>
+  </si>
+  <si>
+    <t>+3 happiness +2 influence</t>
+  </si>
+  <si>
+    <t>+1 happiness for adjacent: mountain, natural wonder, wonder</t>
+  </si>
+  <si>
+    <t>SAWMILL</t>
+  </si>
+  <si>
+    <t>AMPHITHEATER</t>
+  </si>
+  <si>
+    <t>+4 culture</t>
+  </si>
+  <si>
+    <t>+10% production towards wonders</t>
+  </si>
+  <si>
+    <t>BLACKSMITH</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>+1 production to quarters</t>
+  </si>
+  <si>
+    <t>KILN</t>
+  </si>
+  <si>
+    <t>TEMPLE</t>
+  </si>
+  <si>
+    <t>+4 happiness</t>
+  </si>
+  <si>
+    <t>1 relic slot, unlocks Missionaries in this settlement</t>
+  </si>
+  <si>
+    <t>+4 gold +2 influence</t>
+  </si>
+  <si>
+    <t>WHARF</t>
+  </si>
+  <si>
+    <t>Must be placed on coast or navigable river, + 2 ressource slots</t>
   </si>
 </sst>
 </file>
@@ -513,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,7 +602,7 @@
     <col min="4" max="4" width="23.26953125" style="1" customWidth="1"/>
     <col min="5" max="5" width="63.08984375" style="1" customWidth="1"/>
     <col min="6" max="6" width="42.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37.08984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="42.453125" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -608,7 +683,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -623,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -631,7 +706,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -640,13 +715,13 @@
         <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>26</v>
@@ -657,7 +732,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -666,7 +741,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
@@ -680,20 +755,20 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <f>55*320/220</f>
         <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>4</v>
@@ -704,26 +779,26 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <f>55*360/220</f>
         <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>11</v>
@@ -786,10 +861,10 @@
         <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>4</v>
@@ -800,7 +875,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -809,7 +884,7 @@
         <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>20</v>
@@ -823,7 +898,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -832,18 +907,257 @@
         <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="H13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14">
+        <v>90</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>130</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>90</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>90</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18">
+        <v>130</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Notes Column and fixed table size
</commit_message>
<xml_diff>
--- a/Civ7Data.xlsx
+++ b/Civ7Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\git\Civ7CheatSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5D66A5-E259-4258-A178-7305660F6858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424B9E9A-7108-4C0D-9035-1B46324E4F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25710" yWindow="12200" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Must be placed on a river</t>
-  </si>
-  <si>
     <t>GUILDHALL</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>+1 production for adjacent: ressource, wonder</t>
   </si>
   <si>
-    <t>Must be placed on coast adjacent to land</t>
-  </si>
-  <si>
     <t>GRANARY</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
     <t>+1 happiness for adjacent: wonder</t>
   </si>
   <si>
-    <t>Recieves additional bonuses from Pantheon</t>
-  </si>
-  <si>
     <t>MARKET</t>
   </si>
   <si>
@@ -260,16 +251,25 @@
     <t>+4 happiness</t>
   </si>
   <si>
-    <t>1 relic slot, unlocks Missionaries in this settlement</t>
-  </si>
-  <si>
     <t>+4 gold +2 influence</t>
   </si>
   <si>
     <t>WHARF</t>
   </si>
   <si>
-    <t>Must be placed on coast or navigable river, + 2 ressource slots</t>
+    <t>must be placed on a river</t>
+  </si>
+  <si>
+    <t>must be placed on coast adjacent to land</t>
+  </si>
+  <si>
+    <t>gets additional bonuses from Pantheon</t>
+  </si>
+  <si>
+    <t>+ 2 ressource slots; must be placed on coast or navigable river</t>
+  </si>
+  <si>
+    <t>1 relic slot; unlocks missionaries in this settlement</t>
   </si>
 </sst>
 </file>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -675,7 +675,7 @@
         <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>11</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -715,16 +715,16 @@
         <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>11</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -741,7 +741,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
@@ -755,20 +755,20 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <f>55*320/220</f>
         <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>4</v>
@@ -779,26 +779,26 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <f>55*360/220</f>
         <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>11</v>
@@ -852,19 +852,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>4</v>
@@ -875,16 +875,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>20</v>
@@ -898,25 +898,25 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>12</v>
@@ -924,25 +924,25 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>90</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>12</v>
@@ -950,10 +950,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15">
         <v>130</v>
@@ -965,7 +965,7 @@
         <v>19</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>12</v>
@@ -973,19 +973,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>90</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -996,22 +996,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>90</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>12</v>
@@ -1019,19 +1019,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18">
         <v>130</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>4</v>
@@ -1042,22 +1042,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>12</v>
@@ -1065,22 +1065,22 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>12</v>
@@ -1088,22 +1088,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>12</v>
@@ -1111,25 +1111,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>11</v>
@@ -1137,13 +1137,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>23</v>
@@ -1155,7 +1155,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
clearified Age column (unlock age versus ageless), added all missing Antiquity buildings
</commit_message>
<xml_diff>
--- a/Civ7Data.xlsx
+++ b/Civ7Data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\git\Civ7CheatSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7051F32-933E-4173-9A6B-949218F7EF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEDA185-DAFF-4D40-A386-0AE0A7B339D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25710" yWindow="12200" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Experiments" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="118">
   <si>
     <t>Building</t>
   </si>
@@ -105,9 +106,6 @@
     <t>+1 science for adjacent: ressource, wonder</t>
   </si>
   <si>
-    <t>Ageless</t>
-  </si>
-  <si>
     <t>GRISTMILL</t>
   </si>
   <si>
@@ -123,9 +121,6 @@
     <t>GUILDHALL</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>+1 gold for adjacent: coastal terrain, navigable river terrain, wonder</t>
   </si>
   <si>
@@ -291,17 +286,139 @@
     <t>+4 gold</t>
   </si>
   <si>
-    <t>must be placed on a navigable river; land units can move across without needing to embark</t>
+    <t>LIBRARY</t>
+  </si>
+  <si>
+    <t>+2 science</t>
+  </si>
+  <si>
+    <t>2 relic slots</t>
+  </si>
+  <si>
+    <t>ACADEMY</t>
+  </si>
+  <si>
+    <t>3 codex slots</t>
+  </si>
+  <si>
+    <t>FISHING QUAY</t>
+  </si>
+  <si>
+    <t>+1 food to Fishing Boats</t>
+  </si>
+  <si>
+    <t>Must be placed on coast, lake, or navigable river</t>
+  </si>
+  <si>
+    <t>must be placed on navigable river; land units can move across without needing to embark</t>
+  </si>
+  <si>
+    <t>Can the Gristmill be placed on any river</t>
+  </si>
+  <si>
+    <t>Do Barracks keep their 10% production bonus at age transition?</t>
+  </si>
+  <si>
+    <t>Can the Bath be placed on any river -&gt; can be placed on (small) river and navigable river</t>
+  </si>
+  <si>
+    <t>Does Lighthouse keep ist ressource slots at age transition --&gt; no</t>
+  </si>
+  <si>
+    <t>Does Market keep ist ressource slots at age transition --&gt; no</t>
+  </si>
+  <si>
+    <t>after AT with barracks: Courser at 150 needs 8 rounds at 18 prod and initial overprod bonus</t>
+  </si>
+  <si>
+    <t>after AT with barracks: Courser at 150 needs 5 rounds at 33 prod</t>
+  </si>
+  <si>
+    <t>no 10%</t>
+  </si>
+  <si>
+    <t>with 10%</t>
+  </si>
+  <si>
+    <t>after AT no barracks: Courser at 150 needs 12 rounds at 13 prod</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>8 (boosted)</t>
+  </si>
+  <si>
+    <t>Does balcksmith keep bonus to quarters at Age transition? --&gt; no</t>
+  </si>
+  <si>
+    <t>STONECUTTER</t>
+  </si>
+  <si>
+    <t>Is STONECUTTER already available in Antiquity</t>
+  </si>
+  <si>
+    <t>STONECUTTER ageless? -&gt; available only from beginning of exploration</t>
+  </si>
+  <si>
+    <t>SAWMILL ageless -&gt;unlocked in Exploration (machinery), can also be build in Modern</t>
+  </si>
+  <si>
+    <t>hoover keys</t>
+  </si>
+  <si>
+    <t>hoover Text</t>
+  </si>
+  <si>
+    <t>on a river</t>
+  </si>
+  <si>
+    <t>Place on (small) river or a navigable river tile. Can therefore be used to place urban districts on navigable river tiles.</t>
+  </si>
+  <si>
+    <t>Is fishing quay only available when tile to build is available? --&gt;yes</t>
+  </si>
+  <si>
+    <t>Gristmill ageless? -&gt;unlocked in Exploration (machinery), can also be build in Modern</t>
+  </si>
+  <si>
+    <t>ageless</t>
+  </si>
+  <si>
+    <t>Means that this building can also be build in the following ages after it is unlocked. Also means that this building can not be overbuild. So, place carefully, because it is going to stay!</t>
+  </si>
+  <si>
+    <t>The Age in which the building is unlocked and can be build. Only ageless buildings can also be build in the subsequent ages.</t>
+  </si>
+  <si>
+    <t>Antiquity - ageless</t>
+  </si>
+  <si>
+    <t>Exploration - ageless</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,9 +444,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -610,16 +729,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="27.90625" customWidth="1"/>
     <col min="3" max="3" width="26.6328125" customWidth="1"/>
     <col min="4" max="4" width="23.26953125" style="1" customWidth="1"/>
     <col min="5" max="5" width="63.08984375" style="1" customWidth="1"/>
@@ -648,7 +767,7 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>16</v>
@@ -656,45 +775,49 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C2">
-        <v>55</v>
+        <v>195</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C3">
-        <v>175</v>
+        <f>55*360/220</f>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>71</v>
@@ -705,95 +828,94 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C4">
-        <v>55</v>
+        <v>195</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5">
         <v>60</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5">
-        <v>175</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C6">
-        <v>55</v>
+        <v>195</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7">
-        <f>55*320/220</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>12</v>
@@ -801,49 +923,48 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8">
-        <f>55*360/220</f>
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C9">
-        <v>200</v>
+        <v>130</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>12</v>
@@ -851,65 +972,68 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="C10">
-        <v>200</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
+        <v>116</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>4</v>
+        <v>87</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>4</v>
@@ -920,74 +1044,71 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
+        <v>116</v>
+      </c>
+      <c r="C13">
+        <v>55</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="C14">
-        <v>90</v>
+        <v>175</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>12</v>
@@ -995,19 +1116,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -1018,22 +1139,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>12</v>
@@ -1041,22 +1162,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>12</v>
@@ -1064,22 +1188,25 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19">
-        <v>195</v>
+        <v>130</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>63</v>
+        <v>4</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>12</v>
@@ -1087,22 +1214,25 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>65</v>
+        <v>4</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>12</v>
@@ -1110,22 +1240,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>12</v>
@@ -1133,100 +1263,97 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C22" t="s">
-        <v>27</v>
+      <c r="C22">
+        <v>200</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>27</v>
+        <v>116</v>
+      </c>
+      <c r="C23">
+        <v>55</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="C24">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C25">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>80</v>
+        <v>52</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>12</v>
@@ -1234,50 +1361,314 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="C26">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>200</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>200</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29">
+        <v>130</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>175</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
-      <sortCondition ref="B1"/>
+  <autoFilter ref="A1:H30" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H30">
+      <sortCondition ref="A1:A26"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0820759-533E-4E1D-BDF0-8FB06088138D}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="9" max="9" width="17.6328125" customWidth="1"/>
+    <col min="10" max="10" width="10.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6">
+        <f>150/18</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="L6">
+        <f>150/(18*1.1)</f>
+        <v>7.5757575757575752</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <f>150/33</f>
+        <v>4.5454545454545459</v>
+      </c>
+      <c r="L7">
+        <f>150/(33*1.1)</f>
+        <v>4.1322314049586772</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8">
+        <v>12</v>
+      </c>
+      <c r="K8">
+        <f>150/13</f>
+        <v>11.538461538461538</v>
+      </c>
+      <c r="L8" s="2">
+        <f>150/(13*1.1)</f>
+        <v>10.489510489510488</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CBFC140-D462-4BEA-9D0A-BD7084029DBE}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.7265625" customWidth="1"/>
+    <col min="2" max="2" width="48.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added experiment results to xls table
</commit_message>
<xml_diff>
--- a/Civ7Data.xlsx
+++ b/Civ7Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\git\Civ7CheatSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEDA185-DAFF-4D40-A386-0AE0A7B339D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E949C2C-F4E6-422F-B9DF-7CDA2F534B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="12200" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="12200" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1626,8 +1626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CBFC140-D462-4BEA-9D0A-BD7084029DBE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1670,5 +1670,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added exploration and modern buildings
</commit_message>
<xml_diff>
--- a/Civ7Data.xlsx
+++ b/Civ7Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\git\Civ7CheatSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E949C2C-F4E6-422F-B9DF-7CDA2F534B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE97EA6C-3935-4B96-9AEE-788B76E2FFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="12200" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="12200" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Tabelle2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="170">
   <si>
     <t>Building</t>
   </si>
@@ -73,9 +73,6 @@
     <t>+1 production</t>
   </si>
   <si>
-    <t>+1 production to Clay Pits, Mines, and Quarries</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>+4 food</t>
   </si>
   <si>
-    <t>+1 food to Farms, Pastures, and Plantations</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -133,9 +127,6 @@
     <t>SAW PIT</t>
   </si>
   <si>
-    <t>+1 production to Camps, Woodcutters</t>
-  </si>
-  <si>
     <t>+3 production</t>
   </si>
   <si>
@@ -232,9 +223,6 @@
     <t>BLACKSMITH</t>
   </si>
   <si>
-    <t>+1 production to quarters</t>
-  </si>
-  <si>
     <t>KILN</t>
   </si>
   <si>
@@ -259,9 +247,6 @@
     <t>gets additional bonuses from Pantheon</t>
   </si>
   <si>
-    <t>+ 2 ressource slots; must be placed on coast or navigable river</t>
-  </si>
-  <si>
     <t>1 relic slot; unlocks missionaries in this settlement</t>
   </si>
   <si>
@@ -271,15 +256,9 @@
     <t>+3 gold</t>
   </si>
   <si>
-    <t>+ 2 ressource slots; must be placed on coast</t>
-  </si>
-  <si>
     <t>ARENA</t>
   </si>
   <si>
-    <t>+1 happiness on quarters</t>
-  </si>
-  <si>
     <t>ANCIENT BRIDGE</t>
   </si>
   <si>
@@ -304,12 +283,6 @@
     <t>FISHING QUAY</t>
   </si>
   <si>
-    <t>+1 food to Fishing Boats</t>
-  </si>
-  <si>
-    <t>Must be placed on coast, lake, or navigable river</t>
-  </si>
-  <si>
     <t>must be placed on navigable river; land units can move across without needing to embark</t>
   </si>
   <si>
@@ -395,6 +368,189 @@
   </si>
   <si>
     <t>Exploration - ageless</t>
+  </si>
+  <si>
+    <t>city park gives +1 happy on vegetated, all tiles or just the one it is placed on?</t>
+  </si>
+  <si>
+    <t>ARMORER</t>
+  </si>
+  <si>
+    <t>+4 production</t>
+  </si>
+  <si>
+    <t>DUNGEON</t>
+  </si>
+  <si>
+    <t>+3 production +2 influence</t>
+  </si>
+  <si>
+    <t>CANNERY</t>
+  </si>
+  <si>
+    <t>Modern</t>
+  </si>
+  <si>
+    <t>+5 food</t>
+  </si>
+  <si>
+    <t>CITY PARK</t>
+  </si>
+  <si>
+    <t>DEPARTMENT STORE</t>
+  </si>
+  <si>
+    <t>+5 happiness</t>
+  </si>
+  <si>
+    <t>FACTORY</t>
+  </si>
+  <si>
+    <t>+6 production</t>
+  </si>
+  <si>
+    <t>+1 production for adjacent: ressource</t>
+  </si>
+  <si>
+    <t>GROCER</t>
+  </si>
+  <si>
+    <t>Modern - ageless</t>
+  </si>
+  <si>
+    <t>HOSPITAL</t>
+  </si>
+  <si>
+    <t>+15% growth rate</t>
+  </si>
+  <si>
+    <t>IRONWORKS</t>
+  </si>
+  <si>
+    <t>LABORATORY</t>
+  </si>
+  <si>
+    <t>MEDIEVAL BRIDGE</t>
+  </si>
+  <si>
+    <t>MENAGERIE</t>
+  </si>
+  <si>
+    <t>MUSEUM</t>
+  </si>
+  <si>
+    <t>+5 culture</t>
+  </si>
+  <si>
+    <t>OPERA HOUSE</t>
+  </si>
+  <si>
+    <t>+6 culture +3 influence</t>
+  </si>
+  <si>
+    <t>PAVILION</t>
+  </si>
+  <si>
+    <t>PORT</t>
+  </si>
+  <si>
+    <t>+5 gold</t>
+  </si>
+  <si>
+    <t>RADIO STATION</t>
+  </si>
+  <si>
+    <t>+6 happiness +4 influence</t>
+  </si>
+  <si>
+    <t>RAIL STATION</t>
+  </si>
+  <si>
+    <t>+8 gold</t>
+  </si>
+  <si>
+    <t>+10% production towards training units; Upgrades Any Road to Settlements that also have a Rail Station into Railroads; Occupies a full tile.</t>
+  </si>
+  <si>
+    <t>SCHOOLHOUSE</t>
+  </si>
+  <si>
+    <t>STOCK EXCHANGE</t>
+  </si>
+  <si>
+    <t>+6 gold</t>
+  </si>
+  <si>
+    <t>TENEMENT</t>
+  </si>
+  <si>
+    <t>+6 food</t>
+  </si>
+  <si>
+    <t>BANK</t>
+  </si>
+  <si>
+    <t>+3 artifact slots</t>
+  </si>
+  <si>
+    <t>must be placed on coast, lake, or navigable river</t>
+  </si>
+  <si>
+    <t>+ 2 resource slots; must be placed on coast</t>
+  </si>
+  <si>
+    <t>+ 2 resource slots; must be placed on coast adjacent to land</t>
+  </si>
+  <si>
+    <t>+ 2 resource slots; must be placed on coast or navigable river</t>
+  </si>
+  <si>
+    <t>+ 1 resource slot; Allows one type of Factory Resource to be slotted in this Settlement; Must be built in a city connected to the Capital by Railroad.</t>
+  </si>
+  <si>
+    <t>+ 1 resource slot</t>
+  </si>
+  <si>
+    <t>AERODROME</t>
+  </si>
+  <si>
+    <t>+8 production</t>
+  </si>
+  <si>
+    <t>must be placed on Flat Terrain, required to train air units; occupies a full tile</t>
+  </si>
+  <si>
+    <t>+1 food to: Camps, Farms, Fishing Boats, Pastures; Plantations, uncultivated rural tiles</t>
+  </si>
+  <si>
+    <t>+1 food to: Farms, Pastures, and Plantations</t>
+  </si>
+  <si>
+    <t>+1 happiness to: quarters</t>
+  </si>
+  <si>
+    <t>+1 production to: Clay Pits, Mines, and Quarries</t>
+  </si>
+  <si>
+    <t>+1 gold to: quarters</t>
+  </si>
+  <si>
+    <t>+1 production to: Camps, Woodcutters</t>
+  </si>
+  <si>
+    <t>+1 happiness to: Camps and Pastures</t>
+  </si>
+  <si>
+    <t>+1 food to: Fishing Boats</t>
+  </si>
+  <si>
+    <t>+1 production to: quarters</t>
+  </si>
+  <si>
+    <t>+1 happiness on vegetation</t>
+  </si>
+  <si>
+    <t>+1 production to: Mines, Quarries; Woodcutters, Clay Pits</t>
   </si>
 </sst>
 </file>
@@ -729,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -755,239 +911,239 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>195</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <f>55*360/220</f>
         <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <v>195</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="C6">
-        <v>195</v>
+        <v>700</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>78</v>
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7">
-        <v>90</v>
+        <v>195</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>161</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>63</v>
+        <v>163</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="C10">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>11</v>
@@ -995,25 +1151,25 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="C11">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>11</v>
@@ -1021,71 +1177,68 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>4</v>
+        <v>167</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C13">
         <v>55</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>23</v>
+        <v>162</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C14">
-        <v>175</v>
+        <v>600</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>11</v>
@@ -1093,53 +1246,56 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="C15">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>4</v>
+        <v>168</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="C16">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="H16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -1148,186 +1304,180 @@
         <v>200</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="C18">
-        <v>90</v>
+        <v>600</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="C19">
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>4</v>
+        <v>166</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C20">
         <v>90</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="C21">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="C22">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>4</v>
+        <v>160</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C23">
-        <v>55</v>
+        <v>500</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>30</v>
+        <v>159</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>11</v>
@@ -1335,48 +1485,45 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="C26">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>11</v>
@@ -1384,33 +1531,30 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C27">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -1419,53 +1563,53 @@
         <v>200</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="C29">
-        <v>130</v>
+        <v>650</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C30">
-        <v>175</v>
+        <v>90</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>19</v>
@@ -1474,16 +1618,573 @@
         <v>4</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31">
+        <v>130</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32">
+        <v>90</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>200</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>250</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>90</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36">
+        <v>550</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>200</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38">
+        <v>600</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>250</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40">
+        <v>550</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41">
+        <v>700</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42">
+        <v>650</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43">
+        <v>55</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44">
+        <v>175</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45">
+        <v>550</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>200</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47">
+        <v>650</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48">
+        <v>175</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>200</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50">
+        <v>650</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>200</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52">
+        <v>130</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>175</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H30" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H30">
-      <sortCondition ref="A1:A26"/>
+  <autoFilter ref="A1:H53" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H53">
+      <sortCondition ref="A1:A48"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1493,10 +2194,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0820759-533E-4E1D-BDF0-8FB06088138D}">
-  <dimension ref="B2:L15"/>
+  <dimension ref="B2:L16"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1507,39 +2208,39 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" t="s">
         <v>91</v>
       </c>
-      <c r="J5" t="s">
-        <v>100</v>
-      </c>
       <c r="K5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="L5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="J6" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="K6">
         <f>150/18</f>
@@ -1552,7 +2253,7 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="J7">
         <v>5</v>
@@ -1568,7 +2269,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="J8">
         <v>12</v>
@@ -1584,37 +2285,42 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1626,7 +2332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CBFC140-D462-4BEA-9D0A-BD7084029DBE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1638,26 +2344,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1665,7 +2371,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed 'wokr in progress' text
</commit_message>
<xml_diff>
--- a/Civ7Data.xlsx
+++ b/Civ7Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\git\Civ7CheatSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE97EA6C-3935-4B96-9AEE-788B76E2FFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ACF015-94E6-4935-8088-695997768775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25710" yWindow="12200" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -888,7 +888,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>